<commit_message>
attribute name update json tweak
</commit_message>
<xml_diff>
--- a/Minerals data/6.4. Production_of_Mineral_Raw_Materials_of_individual_Countries_by_Minerals.xlsx
+++ b/Minerals data/6.4. Production_of_Mineral_Raw_Materials_of_individual_Countries_by_Minerals.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Sektion IV - Bereich\Bergbau\WMD\WMD 2022\Homepage\01 xlsx fertig zum hochladen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calista\Documents\FIT3179\3179-Data-Visualisation-2\Minerals data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A956A5C-B98D-4458-9DBB-F8C16306D65D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2445" yWindow="2085" windowWidth="27885" windowHeight="8955" tabRatio="863"/>
+    <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="863" firstSheet="23" activeTab="35" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Iron (Fe)" sheetId="4" r:id="rId1"/>
@@ -78,7 +79,20 @@
     <sheet name="Oil Shales" sheetId="64" r:id="rId64"/>
     <sheet name="Uranium (U3O8)" sheetId="66" r:id="rId65"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -640,7 +654,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1314,10 +1328,10 @@
     <xf numFmtId="0" fontId="28" fillId="33" borderId="10" xfId="76" applyFont="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="11" xfId="74" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="34" borderId="11" xfId="74" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="11" xfId="75" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="11" xfId="75" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="33" borderId="10" xfId="75" applyFont="1">
@@ -1332,7 +1346,7 @@
     <xf numFmtId="0" fontId="2" fillId="33" borderId="10" xfId="75" applyFont="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="12" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="12" xfId="76" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="75" applyFont="1">
@@ -1340,83 +1354,83 @@
     </xf>
   </cellXfs>
   <cellStyles count="77">
-    <cellStyle name="20 % - Akzent1 2" xfId="2"/>
-    <cellStyle name="20 % - Akzent1 3" xfId="3"/>
-    <cellStyle name="20 % - Akzent1 4" xfId="4"/>
-    <cellStyle name="20 % - Akzent2 2" xfId="5"/>
-    <cellStyle name="20 % - Akzent2 3" xfId="6"/>
-    <cellStyle name="20 % - Akzent2 4" xfId="7"/>
-    <cellStyle name="20 % - Akzent3 2" xfId="8"/>
-    <cellStyle name="20 % - Akzent3 3" xfId="9"/>
-    <cellStyle name="20 % - Akzent3 4" xfId="10"/>
-    <cellStyle name="20 % - Akzent4 2" xfId="11"/>
-    <cellStyle name="20 % - Akzent4 3" xfId="12"/>
-    <cellStyle name="20 % - Akzent4 4" xfId="13"/>
-    <cellStyle name="20 % - Akzent5 2" xfId="14"/>
-    <cellStyle name="20 % - Akzent5 3" xfId="15"/>
-    <cellStyle name="20 % - Akzent5 4" xfId="16"/>
-    <cellStyle name="20 % - Akzent6 2" xfId="17"/>
-    <cellStyle name="20 % - Akzent6 3" xfId="18"/>
-    <cellStyle name="20 % - Akzent6 4" xfId="19"/>
-    <cellStyle name="40 % - Akzent1 2" xfId="20"/>
-    <cellStyle name="40 % - Akzent1 3" xfId="21"/>
-    <cellStyle name="40 % - Akzent1 4" xfId="22"/>
-    <cellStyle name="40 % - Akzent2 2" xfId="23"/>
-    <cellStyle name="40 % - Akzent2 3" xfId="24"/>
-    <cellStyle name="40 % - Akzent2 4" xfId="25"/>
-    <cellStyle name="40 % - Akzent3 2" xfId="26"/>
-    <cellStyle name="40 % - Akzent3 3" xfId="27"/>
-    <cellStyle name="40 % - Akzent3 4" xfId="28"/>
-    <cellStyle name="40 % - Akzent4 2" xfId="29"/>
-    <cellStyle name="40 % - Akzent4 3" xfId="30"/>
-    <cellStyle name="40 % - Akzent4 4" xfId="31"/>
-    <cellStyle name="40 % - Akzent5 2" xfId="32"/>
-    <cellStyle name="40 % - Akzent5 3" xfId="33"/>
-    <cellStyle name="40 % - Akzent5 4" xfId="34"/>
-    <cellStyle name="40 % - Akzent6 2" xfId="35"/>
-    <cellStyle name="40 % - Akzent6 3" xfId="36"/>
-    <cellStyle name="40 % - Akzent6 4" xfId="37"/>
-    <cellStyle name="60 % - Akzent1 2" xfId="38"/>
-    <cellStyle name="60 % - Akzent2 2" xfId="39"/>
-    <cellStyle name="60 % - Akzent3 2" xfId="40"/>
-    <cellStyle name="60 % - Akzent4 2" xfId="41"/>
-    <cellStyle name="60 % - Akzent5 2" xfId="42"/>
-    <cellStyle name="60 % - Akzent6 2" xfId="43"/>
-    <cellStyle name="Akzent1 2" xfId="44"/>
-    <cellStyle name="Akzent2 2" xfId="45"/>
-    <cellStyle name="Akzent3 2" xfId="46"/>
-    <cellStyle name="Akzent4 2" xfId="47"/>
-    <cellStyle name="Akzent5 2" xfId="48"/>
-    <cellStyle name="Akzent6 2" xfId="49"/>
-    <cellStyle name="Ausgabe 2" xfId="50"/>
-    <cellStyle name="Berechnung 2" xfId="51"/>
-    <cellStyle name="Eingabe 2" xfId="52"/>
-    <cellStyle name="Ergebnis 2" xfId="53"/>
-    <cellStyle name="Erklärender Text 2" xfId="54"/>
-    <cellStyle name="Gut 2" xfId="55"/>
-    <cellStyle name="Neutral 2" xfId="56"/>
-    <cellStyle name="Notiz 2" xfId="57"/>
-    <cellStyle name="Notiz 3" xfId="58"/>
-    <cellStyle name="Notiz 4" xfId="59"/>
-    <cellStyle name="Notiz 5" xfId="60"/>
-    <cellStyle name="Schlecht 2" xfId="61"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Standard 2" xfId="1"/>
-    <cellStyle name="Standard 3" xfId="62"/>
-    <cellStyle name="Standard 4" xfId="63"/>
-    <cellStyle name="Standard 5" xfId="64"/>
-    <cellStyle name="Standard 6" xfId="65"/>
-    <cellStyle name="Stil 1" xfId="66"/>
-    <cellStyle name="Tabelle 1Spalte" xfId="74"/>
-    <cellStyle name="Tabelle allgemein" xfId="75"/>
-    <cellStyle name="Tabelle Kopf" xfId="76"/>
-    <cellStyle name="Überschrift 1 2" xfId="67"/>
-    <cellStyle name="Überschrift 2 2" xfId="68"/>
-    <cellStyle name="Überschrift 3 2" xfId="69"/>
-    <cellStyle name="Überschrift 4 2" xfId="70"/>
-    <cellStyle name="Verknüpfte Zelle 2" xfId="71"/>
-    <cellStyle name="Warnender Text 2" xfId="72"/>
-    <cellStyle name="Zelle überprüfen 2" xfId="73"/>
+    <cellStyle name="20 % - Akzent1 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="20 % - Akzent1 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20 % - Akzent1 4" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="20 % - Akzent2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="20 % - Akzent2 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="20 % - Akzent2 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="20 % - Akzent3 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="20 % - Akzent3 3" xfId="9" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="20 % - Akzent3 4" xfId="10" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="20 % - Akzent4 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="20 % - Akzent4 3" xfId="12" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="20 % - Akzent4 4" xfId="13" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="20 % - Akzent5 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="20 % - Akzent5 3" xfId="15" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="20 % - Akzent5 4" xfId="16" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="20 % - Akzent6 2" xfId="17" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="20 % - Akzent6 3" xfId="18" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="20 % - Akzent6 4" xfId="19" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="40 % - Akzent1 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="40 % - Akzent1 3" xfId="21" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="40 % - Akzent1 4" xfId="22" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="40 % - Akzent2 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="40 % - Akzent2 3" xfId="24" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="40 % - Akzent2 4" xfId="25" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="40 % - Akzent3 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="40 % - Akzent3 3" xfId="27" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="40 % - Akzent3 4" xfId="28" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="40 % - Akzent4 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="40 % - Akzent4 3" xfId="30" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="40 % - Akzent4 4" xfId="31" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="40 % - Akzent5 2" xfId="32" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="40 % - Akzent5 3" xfId="33" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="40 % - Akzent5 4" xfId="34" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="40 % - Akzent6 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="40 % - Akzent6 3" xfId="36" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="40 % - Akzent6 4" xfId="37" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="60 % - Akzent1 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="60 % - Akzent2 2" xfId="39" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="60 % - Akzent3 2" xfId="40" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="60 % - Akzent4 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="60 % - Akzent5 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="60 % - Akzent6 2" xfId="43" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Akzent1 2" xfId="44" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Akzent2 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Akzent3 2" xfId="46" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Akzent4 2" xfId="47" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Akzent5 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Akzent6 2" xfId="49" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Ausgabe 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Berechnung 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Eingabe 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Ergebnis 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Erklärender Text 2" xfId="54" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Gut 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Neutral 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Notiz 2" xfId="57" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Notiz 3" xfId="58" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Notiz 4" xfId="59" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Notiz 5" xfId="60" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="Schlecht 2" xfId="61" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="Standard 3" xfId="62" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="Standard 4" xfId="63" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="Standard 5" xfId="64" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="Standard 6" xfId="65" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Stil 1" xfId="66" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="Tabelle 1Spalte" xfId="74" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="Tabelle allgemein" xfId="75" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="Tabelle Kopf" xfId="76" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="Überschrift 1 2" xfId="67" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="Überschrift 2 2" xfId="68" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="Überschrift 3 2" xfId="69" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="Überschrift 4 2" xfId="70" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
+    <cellStyle name="Verknüpfte Zelle 2" xfId="71" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="Warnender Text 2" xfId="72" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="Zelle überprüfen 2" xfId="73" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
   </cellStyles>
   <dxfs count="633">
     <dxf>
@@ -9030,7 +9044,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="WMD" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="WMD" pivot="0" count="3">
+    <tableStyle name="WMD" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="632"/>
       <tableStyleElement type="headerRow" dxfId="631"/>
       <tableStyleElement type="secondRowStripe" dxfId="630"/>
@@ -9053,1015 +9067,1015 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tab2" displayName="Tab2_" ref="A2:H58" totalsRowShown="0" headerRowDxfId="629" dataDxfId="628" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tab2" displayName="Tab2_" ref="A2:H58" totalsRowShown="0" headerRowDxfId="629" dataDxfId="628" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="627" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="626" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="625" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="624" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="623" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="622" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="621" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="620" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Country" dataDxfId="627" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="unit" dataDxfId="626" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="2016" dataDxfId="625" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="2017" dataDxfId="624" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="2018" dataDxfId="623" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="2019" dataDxfId="622" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="2020" dataDxfId="621" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="data source" dataDxfId="620" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tab2" displayName="Tab2__9" ref="A2:H28" totalsRowShown="0" headerRowDxfId="539" dataDxfId="538" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Tab2" displayName="Tab2__9" ref="A2:H28" totalsRowShown="0" headerRowDxfId="539" dataDxfId="538" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="537" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="536" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="535" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="534" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="533" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="532" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="531" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="530" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Country" dataDxfId="537" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="unit" dataDxfId="536" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="2016" dataDxfId="535" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="2017" dataDxfId="534" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="2018" dataDxfId="533" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="2019" dataDxfId="532" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="2020" dataDxfId="531" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0900-000008000000}" name="data source" dataDxfId="530" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tab2" displayName="Tab2__10" ref="A2:H9" totalsRowShown="0" headerRowDxfId="529" dataDxfId="528" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Tab2" displayName="Tab2__10" ref="A2:H9" totalsRowShown="0" headerRowDxfId="529" dataDxfId="528" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="527" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="526" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="525" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="524" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="523" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="522" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="521" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="520" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="Country" dataDxfId="527" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="unit" dataDxfId="526" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="2016" dataDxfId="525" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="2017" dataDxfId="524" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="2018" dataDxfId="523" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" name="2019" dataDxfId="522" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0A00-000007000000}" name="2020" dataDxfId="521" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0A00-000008000000}" name="data source" dataDxfId="520" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tab2" displayName="Tab2__11" ref="A2:H44" totalsRowShown="0" headerRowDxfId="519" dataDxfId="518" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Tab2" displayName="Tab2__11" ref="A2:H44" totalsRowShown="0" headerRowDxfId="519" dataDxfId="518" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="517" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="516" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="515" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="514" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="513" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="512" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="511" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="510" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="Country" dataDxfId="517" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="unit" dataDxfId="516" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="2016" dataDxfId="515" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0B00-000004000000}" name="2017" dataDxfId="514" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0B00-000005000000}" name="2018" dataDxfId="513" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0B00-000006000000}" name="2019" dataDxfId="512" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0B00-000007000000}" name="2020" dataDxfId="511" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0B00-000008000000}" name="data source" dataDxfId="510" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tab2" displayName="Tab2__12" ref="A2:H23" totalsRowShown="0" headerRowDxfId="509" dataDxfId="508" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Tab2" displayName="Tab2__12" ref="A2:H23" totalsRowShown="0" headerRowDxfId="509" dataDxfId="508" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="507" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="506" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="505" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="504" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="503" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="502" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="501" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="500" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="Country" dataDxfId="507" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="unit" dataDxfId="506" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="2016" dataDxfId="505" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="2017" dataDxfId="504" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="2018" dataDxfId="503" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" name="2019" dataDxfId="502" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" name="2020" dataDxfId="501" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0C00-000008000000}" name="data source" dataDxfId="500" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tab2" displayName="Tab2__13" ref="A2:H12" totalsRowShown="0" headerRowDxfId="499" dataDxfId="498" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Tab2" displayName="Tab2__13" ref="A2:H12" totalsRowShown="0" headerRowDxfId="499" dataDxfId="498" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="497" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="496" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="495" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="494" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="493" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="492" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="491" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="490" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="Country" dataDxfId="497" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="unit" dataDxfId="496" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="2016" dataDxfId="495" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0D00-000004000000}" name="2017" dataDxfId="494" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0D00-000005000000}" name="2018" dataDxfId="493" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0D00-000006000000}" name="2019" dataDxfId="492" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0D00-000007000000}" name="2020" dataDxfId="491" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0D00-000008000000}" name="data source" dataDxfId="490" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tab2" displayName="Tab2__14" ref="A2:H37" totalsRowShown="0" headerRowDxfId="489" dataDxfId="488" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Tab2" displayName="Tab2__14" ref="A2:H37" totalsRowShown="0" headerRowDxfId="489" dataDxfId="488" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="487" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="486" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="485" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="484" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="483" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="482" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="481" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="480" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="Country" dataDxfId="487" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="unit" dataDxfId="486" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="2016" dataDxfId="485" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="2017" dataDxfId="484" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0E00-000005000000}" name="2018" dataDxfId="483" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0E00-000006000000}" name="2019" dataDxfId="482" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0E00-000007000000}" name="2020" dataDxfId="481" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0E00-000008000000}" name="data source" dataDxfId="480" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tab2" displayName="Tab2__15" ref="A2:H14" totalsRowShown="0" headerRowDxfId="479" dataDxfId="478" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="Tab2" displayName="Tab2__15" ref="A2:H14" totalsRowShown="0" headerRowDxfId="479" dataDxfId="478" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="477" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="476" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="475" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="474" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="473" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="472" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="471" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="470" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="Country" dataDxfId="477" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="unit" dataDxfId="476" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0F00-000003000000}" name="2016" dataDxfId="475" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0F00-000004000000}" name="2017" dataDxfId="474" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0F00-000005000000}" name="2018" dataDxfId="473" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0F00-000006000000}" name="2019" dataDxfId="472" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0F00-000007000000}" name="2020" dataDxfId="471" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0F00-000008000000}" name="data source" dataDxfId="470" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Tab2" displayName="Tab2__16" ref="A2:H22" totalsRowShown="0" headerRowDxfId="469" dataDxfId="468" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="Tab2" displayName="Tab2__16" ref="A2:H22" totalsRowShown="0" headerRowDxfId="469" dataDxfId="468" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="467" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="466" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="465" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="464" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="463" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="462" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="461" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="460" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="Country" dataDxfId="467" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="unit" dataDxfId="466" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1000-000003000000}" name="2016" dataDxfId="465" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1000-000004000000}" name="2017" dataDxfId="464" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1000-000005000000}" name="2018" dataDxfId="463" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1000-000006000000}" name="2019" dataDxfId="462" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1000-000007000000}" name="2020" dataDxfId="461" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1000-000008000000}" name="data source" dataDxfId="460" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Tab2" displayName="Tab2__17" ref="A2:H63" totalsRowShown="0" headerRowDxfId="459" dataDxfId="458" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="Tab2" displayName="Tab2__17" ref="A2:H63" totalsRowShown="0" headerRowDxfId="459" dataDxfId="458" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="457" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="456" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="455" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="454" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="453" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="452" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="451" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="450" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="Country" dataDxfId="457" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="unit" dataDxfId="456" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1100-000003000000}" name="2016" dataDxfId="455" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1100-000004000000}" name="2017" dataDxfId="454" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1100-000005000000}" name="2018" dataDxfId="453" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1100-000006000000}" name="2019" dataDxfId="452" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1100-000007000000}" name="2020" dataDxfId="451" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1100-000008000000}" name="data source" dataDxfId="450" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Tab2" displayName="Tab2__18" ref="A2:H9" totalsRowShown="0" headerRowDxfId="449" dataDxfId="448" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF12000000}" name="Tab2" displayName="Tab2__18" ref="A2:H9" totalsRowShown="0" headerRowDxfId="449" dataDxfId="448" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="447" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="446" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="445" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="444" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="443" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="442" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="441" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="440" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1200-000001000000}" name="Country" dataDxfId="447" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1200-000002000000}" name="unit" dataDxfId="446" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1200-000003000000}" name="2016" dataDxfId="445" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1200-000004000000}" name="2017" dataDxfId="444" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1200-000005000000}" name="2018" dataDxfId="443" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1200-000006000000}" name="2019" dataDxfId="442" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1200-000007000000}" name="2020" dataDxfId="441" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1200-000008000000}" name="data source" dataDxfId="440" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tab2" displayName="Tab2__1" ref="A2:H24" totalsRowShown="0" headerRowDxfId="619" dataDxfId="618" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tab2" displayName="Tab2__1" ref="A2:H24" totalsRowShown="0" headerRowDxfId="619" dataDxfId="618" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="617" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="616" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="615" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="614" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="613" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="612" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="611" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="610" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Country" dataDxfId="617" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="unit" dataDxfId="616" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="2016" dataDxfId="615" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="2017" dataDxfId="614" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="2018" dataDxfId="613" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="2019" dataDxfId="612" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="2020" dataDxfId="611" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="data source" dataDxfId="610" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Tab2" displayName="Tab2__19" ref="A2:H8" totalsRowShown="0" headerRowDxfId="439" dataDxfId="438" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{00000000-000C-0000-FFFF-FFFF13000000}" name="Tab2" displayName="Tab2__19" ref="A2:H8" totalsRowShown="0" headerRowDxfId="439" dataDxfId="438" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="437" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="436" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="435" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="434" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="433" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="432" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="431" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="430" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1300-000001000000}" name="Country" dataDxfId="437" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1300-000002000000}" name="unit" dataDxfId="436" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1300-000003000000}" name="2016" dataDxfId="435" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1300-000004000000}" name="2017" dataDxfId="434" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1300-000005000000}" name="2018" dataDxfId="433" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1300-000006000000}" name="2019" dataDxfId="432" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1300-000007000000}" name="2020" dataDxfId="431" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1300-000008000000}" name="data source" dataDxfId="430" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Tab2" displayName="Tab2__20" ref="A2:H52" totalsRowShown="0" headerRowDxfId="429" dataDxfId="428" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{00000000-000C-0000-FFFF-FFFF14000000}" name="Tab2" displayName="Tab2__20" ref="A2:H52" totalsRowShown="0" headerRowDxfId="429" dataDxfId="428" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="427" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="426" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="425" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="424" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="423" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="422" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="421" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="420" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1400-000001000000}" name="Country" dataDxfId="427" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1400-000002000000}" name="unit" dataDxfId="426" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1400-000003000000}" name="2016" dataDxfId="425" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1400-000004000000}" name="2017" dataDxfId="424" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1400-000005000000}" name="2018" dataDxfId="423" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1400-000006000000}" name="2019" dataDxfId="422" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1400-000007000000}" name="2020" dataDxfId="421" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1400-000008000000}" name="data source" dataDxfId="420" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Tab2" displayName="Tab2__21" ref="A2:H15" totalsRowShown="0" headerRowDxfId="419" dataDxfId="418" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{00000000-000C-0000-FFFF-FFFF15000000}" name="Tab2" displayName="Tab2__21" ref="A2:H15" totalsRowShown="0" headerRowDxfId="419" dataDxfId="418" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="417" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="416" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="415" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="414" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="413" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="412" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="411" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="410" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1500-000001000000}" name="Country" dataDxfId="417" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1500-000002000000}" name="unit" dataDxfId="416" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1500-000003000000}" name="2016" dataDxfId="415" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1500-000004000000}" name="2017" dataDxfId="414" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1500-000005000000}" name="2018" dataDxfId="413" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1500-000006000000}" name="2019" dataDxfId="412" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1500-000007000000}" name="2020" dataDxfId="411" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1500-000008000000}" name="data source" dataDxfId="410" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Tab2" displayName="Tab2__22" ref="A2:H13" totalsRowShown="0" headerRowDxfId="409" dataDxfId="408" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{00000000-000C-0000-FFFF-FFFF16000000}" name="Tab2" displayName="Tab2__22" ref="A2:H13" totalsRowShown="0" headerRowDxfId="409" dataDxfId="408" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="407" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="406" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="405" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="404" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="403" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="402" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="401" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="400" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1600-000001000000}" name="Country" dataDxfId="407" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1600-000002000000}" name="unit" dataDxfId="406" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1600-000003000000}" name="2016" dataDxfId="405" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1600-000004000000}" name="2017" dataDxfId="404" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1600-000005000000}" name="2018" dataDxfId="403" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1600-000006000000}" name="2019" dataDxfId="402" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1600-000007000000}" name="2020" dataDxfId="401" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1600-000008000000}" name="data source" dataDxfId="400" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Tab2" displayName="Tab2__23" ref="A2:H12" totalsRowShown="0" headerRowDxfId="399" dataDxfId="398" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{00000000-000C-0000-FFFF-FFFF17000000}" name="Tab2" displayName="Tab2__23" ref="A2:H12" totalsRowShown="0" headerRowDxfId="399" dataDxfId="398" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="397" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="396" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="395" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="394" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="393" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="392" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="391" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="390" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1700-000001000000}" name="Country" dataDxfId="397" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1700-000002000000}" name="unit" dataDxfId="396" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1700-000003000000}" name="2016" dataDxfId="395" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1700-000004000000}" name="2017" dataDxfId="394" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1700-000005000000}" name="2018" dataDxfId="393" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1700-000006000000}" name="2019" dataDxfId="392" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1700-000007000000}" name="2020" dataDxfId="391" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1700-000008000000}" name="data source" dataDxfId="390" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Tab2" displayName="Tab2__24" ref="A2:H11" totalsRowShown="0" headerRowDxfId="389" dataDxfId="388" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{00000000-000C-0000-FFFF-FFFF18000000}" name="Tab2" displayName="Tab2__24" ref="A2:H11" totalsRowShown="0" headerRowDxfId="389" dataDxfId="388" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="387" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="386" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="385" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="384" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="383" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="382" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="381" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="380" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1800-000001000000}" name="Country" dataDxfId="387" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1800-000002000000}" name="unit" dataDxfId="386" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1800-000003000000}" name="2016" dataDxfId="385" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1800-000004000000}" name="2017" dataDxfId="384" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1800-000005000000}" name="2018" dataDxfId="383" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1800-000006000000}" name="2019" dataDxfId="382" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1800-000007000000}" name="2020" dataDxfId="381" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1800-000008000000}" name="data source" dataDxfId="380" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Tab2" displayName="Tab2__25" ref="A2:H21" totalsRowShown="0" headerRowDxfId="379" dataDxfId="378" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{00000000-000C-0000-FFFF-FFFF19000000}" name="Tab2" displayName="Tab2__25" ref="A2:H21" totalsRowShown="0" headerRowDxfId="379" dataDxfId="378" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="377" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="376" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="375" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="374" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="373" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="372" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="371" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="370" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1900-000001000000}" name="Country" dataDxfId="377" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1900-000002000000}" name="unit" dataDxfId="376" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1900-000003000000}" name="2016" dataDxfId="375" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1900-000004000000}" name="2017" dataDxfId="374" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1900-000005000000}" name="2018" dataDxfId="373" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1900-000006000000}" name="2019" dataDxfId="372" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1900-000007000000}" name="2020" dataDxfId="371" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1900-000008000000}" name="data source" dataDxfId="370" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="Tab2" displayName="Tab2__26" ref="A2:H11" totalsRowShown="0" headerRowDxfId="369" dataDxfId="368" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{00000000-000C-0000-FFFF-FFFF1A000000}" name="Tab2" displayName="Tab2__26" ref="A2:H11" totalsRowShown="0" headerRowDxfId="369" dataDxfId="368" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="367" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="366" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="365" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="364" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="363" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="362" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="361" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="360" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1A00-000001000000}" name="Country" dataDxfId="367" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1A00-000002000000}" name="unit" dataDxfId="366" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1A00-000003000000}" name="2016" dataDxfId="365" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1A00-000004000000}" name="2017" dataDxfId="364" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1A00-000005000000}" name="2018" dataDxfId="363" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1A00-000006000000}" name="2019" dataDxfId="362" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1A00-000007000000}" name="2020" dataDxfId="361" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1A00-000008000000}" name="data source" dataDxfId="360" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Tab2" displayName="Tab2__27" ref="A2:H28" totalsRowShown="0" headerRowDxfId="359" dataDxfId="358" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{00000000-000C-0000-FFFF-FFFF1B000000}" name="Tab2" displayName="Tab2__27" ref="A2:H28" totalsRowShown="0" headerRowDxfId="359" dataDxfId="358" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="357" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="356" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="355" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="354" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="353" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="352" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="351" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="350" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1B00-000001000000}" name="Country" dataDxfId="357" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1B00-000002000000}" name="unit" dataDxfId="356" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1B00-000003000000}" name="2016" dataDxfId="355" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1B00-000004000000}" name="2017" dataDxfId="354" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1B00-000005000000}" name="2018" dataDxfId="353" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1B00-000006000000}" name="2019" dataDxfId="352" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1B00-000007000000}" name="2020" dataDxfId="351" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1B00-000008000000}" name="data source" dataDxfId="350" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="Tab2" displayName="Tab2__28" ref="A2:H59" totalsRowShown="0" headerRowDxfId="349" dataDxfId="348" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{00000000-000C-0000-FFFF-FFFF1C000000}" name="Tab2" displayName="Tab2__28" ref="A2:H59" totalsRowShown="0" headerRowDxfId="349" dataDxfId="348" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="347" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="346" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="345" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="344" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="343" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="342" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="341" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="340" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1C00-000001000000}" name="Country" dataDxfId="347" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1C00-000002000000}" name="unit" dataDxfId="346" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1C00-000003000000}" name="2016" dataDxfId="345" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1C00-000004000000}" name="2017" dataDxfId="344" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1C00-000005000000}" name="2018" dataDxfId="343" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1C00-000006000000}" name="2019" dataDxfId="342" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1C00-000007000000}" name="2020" dataDxfId="341" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1C00-000008000000}" name="data source" dataDxfId="340" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tab2" displayName="Tab2__2" ref="A2:H24" totalsRowShown="0" headerRowDxfId="609" dataDxfId="608" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tab2" displayName="Tab2__2" ref="A2:H24" totalsRowShown="0" headerRowDxfId="609" dataDxfId="608" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="607" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="606" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="605" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="604" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="603" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="602" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="601" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="600" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Country" dataDxfId="607" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="unit" dataDxfId="606" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="2016" dataDxfId="605" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="2017" dataDxfId="604" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="2018" dataDxfId="603" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="2019" dataDxfId="602" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="2020" dataDxfId="601" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="data source" dataDxfId="600" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="Tab2" displayName="Tab2__29" ref="A2:H103" totalsRowShown="0" headerRowDxfId="339" dataDxfId="338" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{00000000-000C-0000-FFFF-FFFF1D000000}" name="Tab2" displayName="Tab2__29" ref="A2:H103" totalsRowShown="0" headerRowDxfId="339" dataDxfId="338" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="337" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="336" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="335" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="334" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="333" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="332" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="331" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="330" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1D00-000001000000}" name="Country" dataDxfId="337" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1D00-000002000000}" name="unit" dataDxfId="336" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1D00-000003000000}" name="2016" dataDxfId="335" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1D00-000004000000}" name="2017" dataDxfId="334" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1D00-000005000000}" name="2018" dataDxfId="333" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1D00-000006000000}" name="2019" dataDxfId="332" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1D00-000007000000}" name="2020" dataDxfId="331" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1D00-000008000000}" name="data source" dataDxfId="330" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="Tab2" displayName="Tab2__30" ref="A2:H14" totalsRowShown="0" headerRowDxfId="329" dataDxfId="328" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{00000000-000C-0000-FFFF-FFFF1E000000}" name="Tab2" displayName="Tab2__30" ref="A2:H14" totalsRowShown="0" headerRowDxfId="329" dataDxfId="328" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="327" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="326" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="325" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="324" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="323" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="322" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="321" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="320" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1E00-000001000000}" name="Country" dataDxfId="327" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1E00-000002000000}" name="unit" dataDxfId="326" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1E00-000003000000}" name="2016" dataDxfId="325" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1E00-000004000000}" name="2017" dataDxfId="324" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1E00-000005000000}" name="2018" dataDxfId="323" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1E00-000006000000}" name="2019" dataDxfId="322" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1E00-000007000000}" name="2020" dataDxfId="321" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1E00-000008000000}" name="data source" dataDxfId="320" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="32" name="Tab2" displayName="Tab2__31" ref="A2:H14" totalsRowShown="0" headerRowDxfId="319" dataDxfId="318" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{00000000-000C-0000-FFFF-FFFF1F000000}" name="Tab2" displayName="Tab2__31" ref="A2:H14" totalsRowShown="0" headerRowDxfId="319" dataDxfId="318" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="317" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="316" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="315" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="314" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="313" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="312" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="311" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="310" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1F00-000001000000}" name="Country" dataDxfId="317" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1F00-000002000000}" name="unit" dataDxfId="316" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1F00-000003000000}" name="2016" dataDxfId="315" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1F00-000004000000}" name="2017" dataDxfId="314" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1F00-000005000000}" name="2018" dataDxfId="313" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1F00-000006000000}" name="2019" dataDxfId="312" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1F00-000007000000}" name="2020" dataDxfId="311" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1F00-000008000000}" name="data source" dataDxfId="310" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table33.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="33" name="Tab2" displayName="Tab2__32" ref="A2:H8" totalsRowShown="0" headerRowDxfId="309" dataDxfId="308" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{00000000-000C-0000-FFFF-FFFF20000000}" name="Tab2" displayName="Tab2__32" ref="A2:H8" totalsRowShown="0" headerRowDxfId="309" dataDxfId="308" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="307" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="306" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="305" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="304" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="303" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="302" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="301" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="300" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2000-000001000000}" name="Country" dataDxfId="307" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2000-000002000000}" name="unit" dataDxfId="306" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2000-000003000000}" name="2016" dataDxfId="305" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2000-000004000000}" name="2017" dataDxfId="304" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2000-000005000000}" name="2018" dataDxfId="303" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2000-000006000000}" name="2019" dataDxfId="302" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-2000-000007000000}" name="2020" dataDxfId="301" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-2000-000008000000}" name="data source" dataDxfId="300" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table34.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="34" name="Tab2" displayName="Tab2__33" ref="A2:H74" totalsRowShown="0" headerRowDxfId="299" dataDxfId="298" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{00000000-000C-0000-FFFF-FFFF21000000}" name="Tab2" displayName="Tab2__33" ref="A2:H74" totalsRowShown="0" headerRowDxfId="299" dataDxfId="298" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="297" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="296" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="295" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="294" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="293" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="292" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="291" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="290" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2100-000001000000}" name="Country" dataDxfId="297" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2100-000002000000}" name="unit" dataDxfId="296" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2100-000003000000}" name="2016" dataDxfId="295" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2100-000004000000}" name="2017" dataDxfId="294" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2100-000005000000}" name="2018" dataDxfId="293" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2100-000006000000}" name="2019" dataDxfId="292" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-2100-000007000000}" name="2020" dataDxfId="291" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-2100-000008000000}" name="data source" dataDxfId="290" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table35.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="35" name="Tab2" displayName="Tab2__34" ref="A2:H8" totalsRowShown="0" headerRowDxfId="289" dataDxfId="288" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{00000000-000C-0000-FFFF-FFFF22000000}" name="Tab2" displayName="Tab2__34" ref="A2:H8" totalsRowShown="0" headerRowDxfId="289" dataDxfId="288" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="287" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="286" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="285" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="284" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="283" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="282" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="281" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="280" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2200-000001000000}" name="Country" dataDxfId="287" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2200-000002000000}" name="unit" dataDxfId="286" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2200-000003000000}" name="2016" dataDxfId="285" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2200-000004000000}" name="2017" dataDxfId="284" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2200-000005000000}" name="2018" dataDxfId="283" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2200-000006000000}" name="2019" dataDxfId="282" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-2200-000007000000}" name="2020" dataDxfId="281" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-2200-000008000000}" name="data source" dataDxfId="280" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table36.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="36" name="Tab2" displayName="Tab2__35" ref="A2:H35" totalsRowShown="0" headerRowDxfId="279" dataDxfId="278" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="36" xr:uid="{00000000-000C-0000-FFFF-FFFF23000000}" name="Tab2" displayName="Tab2__35" ref="A2:H35" totalsRowShown="0" headerRowDxfId="279" dataDxfId="278" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="277" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="276" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="275" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="274" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="273" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="272" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="271" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="270" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2300-000001000000}" name="Country" dataDxfId="277" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2300-000002000000}" name="unit" dataDxfId="276" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2300-000003000000}" name="2016" dataDxfId="275" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2300-000004000000}" name="2017" dataDxfId="274" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2300-000005000000}" name="2018" dataDxfId="273" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2300-000006000000}" name="2019" dataDxfId="272" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-2300-000007000000}" name="2020" dataDxfId="271" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-2300-000008000000}" name="data source" dataDxfId="270" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table37.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="37" name="Tab2" displayName="Tab2__36" ref="A2:H53" totalsRowShown="0" headerRowDxfId="269" dataDxfId="268" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="37" xr:uid="{00000000-000C-0000-FFFF-FFFF24000000}" name="Tab2" displayName="Tab2__36" ref="A2:H53" totalsRowShown="0" headerRowDxfId="269" dataDxfId="268" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="267" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="266" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="265" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="264" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="263" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="262" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="261" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="260" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2400-000001000000}" name="Country" dataDxfId="267" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2400-000002000000}" name="unit" dataDxfId="266" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2400-000003000000}" name="2016" dataDxfId="265" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2400-000004000000}" name="2017" dataDxfId="264" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2400-000005000000}" name="2018" dataDxfId="263" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2400-000006000000}" name="2019" dataDxfId="262" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-2400-000007000000}" name="2020" dataDxfId="261" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-2400-000008000000}" name="data source" dataDxfId="260" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table38.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="38" name="Tab2" displayName="Tab2__37" ref="A2:H13" totalsRowShown="0" headerRowDxfId="259" dataDxfId="258" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="38" xr:uid="{00000000-000C-0000-FFFF-FFFF25000000}" name="Tab2" displayName="Tab2__37" ref="A2:H13" totalsRowShown="0" headerRowDxfId="259" dataDxfId="258" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="257" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="256" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="255" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="254" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="253" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="252" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="251" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="250" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2500-000001000000}" name="Country" dataDxfId="257" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2500-000002000000}" name="unit" dataDxfId="256" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2500-000003000000}" name="2016" dataDxfId="255" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2500-000004000000}" name="2017" dataDxfId="254" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2500-000005000000}" name="2018" dataDxfId="253" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2500-000006000000}" name="2019" dataDxfId="252" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-2500-000007000000}" name="2020" dataDxfId="251" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-2500-000008000000}" name="data source" dataDxfId="250" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table39.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="39" name="Tab2" displayName="Tab2__38" ref="A2:H25" totalsRowShown="0" headerRowDxfId="249" dataDxfId="248" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="39" xr:uid="{00000000-000C-0000-FFFF-FFFF26000000}" name="Tab2" displayName="Tab2__38" ref="A2:H25" totalsRowShown="0" headerRowDxfId="249" dataDxfId="248" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="247" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="246" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="245" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="244" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="243" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="242" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="241" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="240" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2600-000001000000}" name="Country" dataDxfId="247" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2600-000002000000}" name="unit" dataDxfId="246" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2600-000003000000}" name="2016" dataDxfId="245" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2600-000004000000}" name="2017" dataDxfId="244" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2600-000005000000}" name="2018" dataDxfId="243" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2600-000006000000}" name="2019" dataDxfId="242" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-2600-000007000000}" name="2020" dataDxfId="241" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-2600-000008000000}" name="data source" dataDxfId="240" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tab2" displayName="Tab2__3" ref="A2:H41" totalsRowShown="0" headerRowDxfId="599" dataDxfId="598" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tab2" displayName="Tab2__3" ref="A2:H41" totalsRowShown="0" headerRowDxfId="599" dataDxfId="598" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="597" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="596" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="595" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="594" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="593" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="592" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="591" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="590" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Country" dataDxfId="597" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="unit" dataDxfId="596" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="2016" dataDxfId="595" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="2017" dataDxfId="594" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="2018" dataDxfId="593" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="2019" dataDxfId="592" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="2020" dataDxfId="591" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="data source" dataDxfId="590" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table40.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="40" name="Tab2" displayName="Tab2__39" ref="A2:H25" totalsRowShown="0" headerRowDxfId="239" dataDxfId="238" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="40" xr:uid="{00000000-000C-0000-FFFF-FFFF27000000}" name="Tab2" displayName="Tab2__39" ref="A2:H25" totalsRowShown="0" headerRowDxfId="239" dataDxfId="238" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="237" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="236" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="235" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="234" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="233" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="232" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="231" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="230" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2700-000001000000}" name="Country" dataDxfId="237" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2700-000002000000}" name="unit" dataDxfId="236" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2700-000003000000}" name="2016" dataDxfId="235" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2700-000004000000}" name="2017" dataDxfId="234" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2700-000005000000}" name="2018" dataDxfId="233" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2700-000006000000}" name="2019" dataDxfId="232" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-2700-000007000000}" name="2020" dataDxfId="231" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-2700-000008000000}" name="data source" dataDxfId="230" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table41.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="41" name="Tab2" displayName="Tab2__40" ref="A2:H27" totalsRowShown="0" headerRowDxfId="229" dataDxfId="228" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="41" xr:uid="{00000000-000C-0000-FFFF-FFFF28000000}" name="Tab2" displayName="Tab2__40" ref="A2:H27" totalsRowShown="0" headerRowDxfId="229" dataDxfId="228" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="227" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="226" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="225" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="224" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="223" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="222" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="221" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="220" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2800-000001000000}" name="Country" dataDxfId="227" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2800-000002000000}" name="unit" dataDxfId="226" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2800-000003000000}" name="2016" dataDxfId="225" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2800-000004000000}" name="2017" dataDxfId="224" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2800-000005000000}" name="2018" dataDxfId="223" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2800-000006000000}" name="2019" dataDxfId="222" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-2800-000007000000}" name="2020" dataDxfId="221" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-2800-000008000000}" name="data source" dataDxfId="220" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table42.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="42" name="Tab2" displayName="Tab2__41" ref="A2:H51" totalsRowShown="0" headerRowDxfId="219" dataDxfId="218" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="42" xr:uid="{00000000-000C-0000-FFFF-FFFF29000000}" name="Tab2" displayName="Tab2__41" ref="A2:H51" totalsRowShown="0" headerRowDxfId="219" dataDxfId="218" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="217" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="216" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="215" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="214" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="213" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="212" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="211" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="210" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2900-000001000000}" name="Country" dataDxfId="217" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2900-000002000000}" name="unit" dataDxfId="216" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2900-000003000000}" name="2016" dataDxfId="215" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2900-000004000000}" name="2017" dataDxfId="214" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2900-000005000000}" name="2018" dataDxfId="213" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2900-000006000000}" name="2019" dataDxfId="212" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-2900-000007000000}" name="2020" dataDxfId="211" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-2900-000008000000}" name="data source" dataDxfId="210" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table43.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="43" name="Tab2" displayName="Tab2__42" ref="A2:H29" totalsRowShown="0" headerRowDxfId="209" dataDxfId="208" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="43" xr:uid="{00000000-000C-0000-FFFF-FFFF2A000000}" name="Tab2" displayName="Tab2__42" ref="A2:H29" totalsRowShown="0" headerRowDxfId="209" dataDxfId="208" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="207" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="206" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="205" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="204" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="203" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="202" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="201" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="200" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2A00-000001000000}" name="Country" dataDxfId="207" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2A00-000002000000}" name="unit" dataDxfId="206" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2A00-000003000000}" name="2016" dataDxfId="205" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2A00-000004000000}" name="2017" dataDxfId="204" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2A00-000005000000}" name="2018" dataDxfId="203" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2A00-000006000000}" name="2019" dataDxfId="202" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-2A00-000007000000}" name="2020" dataDxfId="201" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-2A00-000008000000}" name="data source" dataDxfId="200" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table44.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="44" name="Tab2" displayName="Tab2__43" ref="A2:H23" totalsRowShown="0" headerRowDxfId="199" dataDxfId="198" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="44" xr:uid="{00000000-000C-0000-FFFF-FFFF2B000000}" name="Tab2" displayName="Tab2__43" ref="A2:H23" totalsRowShown="0" headerRowDxfId="199" dataDxfId="198" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="197" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="196" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="195" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="194" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="193" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="192" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="191" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="190" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2B00-000001000000}" name="Country" dataDxfId="197" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2B00-000002000000}" name="unit" dataDxfId="196" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2B00-000003000000}" name="2016" dataDxfId="195" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2B00-000004000000}" name="2017" dataDxfId="194" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2B00-000005000000}" name="2018" dataDxfId="193" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2B00-000006000000}" name="2019" dataDxfId="192" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-2B00-000007000000}" name="2020" dataDxfId="191" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-2B00-000008000000}" name="data source" dataDxfId="190" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table45.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="45" name="Tab2" displayName="Tab2__44" ref="A2:H81" totalsRowShown="0" headerRowDxfId="189" dataDxfId="188" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="45" xr:uid="{00000000-000C-0000-FFFF-FFFF2C000000}" name="Tab2" displayName="Tab2__44" ref="A2:H81" totalsRowShown="0" headerRowDxfId="189" dataDxfId="188" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="187" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="186" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="185" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="184" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="183" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="182" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="181" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="180" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2C00-000001000000}" name="Country" dataDxfId="187" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2C00-000002000000}" name="unit" dataDxfId="186" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2C00-000003000000}" name="2016" dataDxfId="185" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2C00-000004000000}" name="2017" dataDxfId="184" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2C00-000005000000}" name="2018" dataDxfId="183" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2C00-000006000000}" name="2019" dataDxfId="182" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-2C00-000007000000}" name="2020" dataDxfId="181" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-2C00-000008000000}" name="data source" dataDxfId="180" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table46.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="46" name="Tab2" displayName="Tab2__45" ref="A2:H61" totalsRowShown="0" headerRowDxfId="179" dataDxfId="178" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="46" xr:uid="{00000000-000C-0000-FFFF-FFFF2D000000}" name="Tab2" displayName="Tab2__45" ref="A2:H61" totalsRowShown="0" headerRowDxfId="179" dataDxfId="178" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="177" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="176" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="175" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="174" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="173" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="172" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="171" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="170" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2D00-000001000000}" name="Country" dataDxfId="177" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2D00-000002000000}" name="unit" dataDxfId="176" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2D00-000003000000}" name="2016" dataDxfId="175" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2D00-000004000000}" name="2017" dataDxfId="174" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2D00-000005000000}" name="2018" dataDxfId="173" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2D00-000006000000}" name="2019" dataDxfId="172" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-2D00-000007000000}" name="2020" dataDxfId="171" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-2D00-000008000000}" name="data source" dataDxfId="170" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table47.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="47" name="Tab2" displayName="Tab2__46" ref="A2:H28" totalsRowShown="0" headerRowDxfId="169" dataDxfId="168" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="47" xr:uid="{00000000-000C-0000-FFFF-FFFF2E000000}" name="Tab2" displayName="Tab2__46" ref="A2:H28" totalsRowShown="0" headerRowDxfId="169" dataDxfId="168" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="167" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="166" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="165" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="164" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="163" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="162" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="161" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="160" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2E00-000001000000}" name="Country" dataDxfId="167" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2E00-000002000000}" name="unit" dataDxfId="166" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2E00-000003000000}" name="2016" dataDxfId="165" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2E00-000004000000}" name="2017" dataDxfId="164" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2E00-000005000000}" name="2018" dataDxfId="163" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2E00-000006000000}" name="2019" dataDxfId="162" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-2E00-000007000000}" name="2020" dataDxfId="161" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-2E00-000008000000}" name="data source" dataDxfId="160" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table48.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="48" name="Tab2" displayName="Tab2__47" ref="A2:H19" totalsRowShown="0" headerRowDxfId="159" dataDxfId="158" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="48" xr:uid="{00000000-000C-0000-FFFF-FFFF2F000000}" name="Tab2" displayName="Tab2__47" ref="A2:H19" totalsRowShown="0" headerRowDxfId="159" dataDxfId="158" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="157" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="156" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="155" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="154" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="153" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="152" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="151" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="150" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2F00-000001000000}" name="Country" dataDxfId="157" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2F00-000002000000}" name="unit" dataDxfId="156" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2F00-000003000000}" name="2016" dataDxfId="155" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2F00-000004000000}" name="2017" dataDxfId="154" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2F00-000005000000}" name="2018" dataDxfId="153" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2F00-000006000000}" name="2019" dataDxfId="152" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-2F00-000007000000}" name="2020" dataDxfId="151" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-2F00-000008000000}" name="data source" dataDxfId="150" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table49.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="49" name="Tab2" displayName="Tab2__48" ref="A2:H42" totalsRowShown="0" headerRowDxfId="149" dataDxfId="148" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="49" xr:uid="{00000000-000C-0000-FFFF-FFFF30000000}" name="Tab2" displayName="Tab2__48" ref="A2:H42" totalsRowShown="0" headerRowDxfId="149" dataDxfId="148" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="147" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="146" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="145" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="144" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="143" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="142" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="141" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="140" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-3000-000001000000}" name="Country" dataDxfId="147" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-3000-000002000000}" name="unit" dataDxfId="146" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-3000-000003000000}" name="2016" dataDxfId="145" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-3000-000004000000}" name="2017" dataDxfId="144" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-3000-000005000000}" name="2018" dataDxfId="143" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-3000-000006000000}" name="2019" dataDxfId="142" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-3000-000007000000}" name="2020" dataDxfId="141" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-3000-000008000000}" name="data source" dataDxfId="140" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tab2" displayName="Tab2__4" ref="A2:H20" totalsRowShown="0" headerRowDxfId="589" dataDxfId="588" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tab2" displayName="Tab2__4" ref="A2:H20" totalsRowShown="0" headerRowDxfId="589" dataDxfId="588" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="587" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="586" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="585" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="584" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="583" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="582" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="581" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="580" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Country" dataDxfId="587" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="unit" dataDxfId="586" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="2016" dataDxfId="585" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="2017" dataDxfId="584" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="2018" dataDxfId="583" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="2019" dataDxfId="582" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="2020" dataDxfId="581" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="data source" dataDxfId="580" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table50.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="50" name="Tab2" displayName="Tab2__49" ref="A2:H20" totalsRowShown="0" headerRowDxfId="139" dataDxfId="138" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="50" xr:uid="{00000000-000C-0000-FFFF-FFFF31000000}" name="Tab2" displayName="Tab2__49" ref="A2:H20" totalsRowShown="0" headerRowDxfId="139" dataDxfId="138" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="137" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="136" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="135" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="134" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="133" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="132" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="131" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="130" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-3100-000001000000}" name="Country" dataDxfId="137" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-3100-000002000000}" name="unit" dataDxfId="136" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-3100-000003000000}" name="2016" dataDxfId="135" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-3100-000004000000}" name="2017" dataDxfId="134" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-3100-000005000000}" name="2018" dataDxfId="133" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-3100-000006000000}" name="2019" dataDxfId="132" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-3100-000007000000}" name="2020" dataDxfId="131" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-3100-000008000000}" name="data source" dataDxfId="130" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table51.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="51" name="Tab2" displayName="Tab2__50" ref="A2:H104" totalsRowShown="0" headerRowDxfId="129" dataDxfId="128" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="51" xr:uid="{00000000-000C-0000-FFFF-FFFF32000000}" name="Tab2" displayName="Tab2__50" ref="A2:H104" totalsRowShown="0" headerRowDxfId="129" dataDxfId="128" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="127" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="126" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="125" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="124" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="123" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="122" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="121" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="120" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-3200-000001000000}" name="Country" dataDxfId="127" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-3200-000002000000}" name="unit" dataDxfId="126" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-3200-000003000000}" name="2016" dataDxfId="125" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-3200-000004000000}" name="2017" dataDxfId="124" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-3200-000005000000}" name="2018" dataDxfId="123" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-3200-000006000000}" name="2019" dataDxfId="122" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-3200-000007000000}" name="2020" dataDxfId="121" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-3200-000008000000}" name="data source" dataDxfId="120" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table52.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="52" name="Tab2" displayName="Tab2__51" ref="A2:H57" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="52" xr:uid="{00000000-000C-0000-FFFF-FFFF33000000}" name="Tab2" displayName="Tab2__51" ref="A2:H57" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="117" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="116" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="115" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="114" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="113" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="112" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="111" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="110" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-3300-000001000000}" name="Country" dataDxfId="117" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-3300-000002000000}" name="unit" dataDxfId="116" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-3300-000003000000}" name="2016" dataDxfId="115" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-3300-000004000000}" name="2017" dataDxfId="114" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-3300-000005000000}" name="2018" dataDxfId="113" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-3300-000006000000}" name="2019" dataDxfId="112" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-3300-000007000000}" name="2020" dataDxfId="111" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-3300-000008000000}" name="data source" dataDxfId="110" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table53.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="53" name="Tab2" displayName="Tab2__52" ref="A2:H40" totalsRowShown="0" headerRowDxfId="109" dataDxfId="108" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="53" xr:uid="{00000000-000C-0000-FFFF-FFFF34000000}" name="Tab2" displayName="Tab2__52" ref="A2:H40" totalsRowShown="0" headerRowDxfId="109" dataDxfId="108" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="107" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="106" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="105" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="104" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="103" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="102" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="101" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="100" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-3400-000001000000}" name="Country" dataDxfId="107" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-3400-000002000000}" name="unit" dataDxfId="106" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-3400-000003000000}" name="2016" dataDxfId="105" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-3400-000004000000}" name="2017" dataDxfId="104" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-3400-000005000000}" name="2018" dataDxfId="103" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-3400-000006000000}" name="2019" dataDxfId="102" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-3400-000007000000}" name="2020" dataDxfId="101" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-3400-000008000000}" name="data source" dataDxfId="100" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table54.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="54" name="Tab2" displayName="Tab2__53" ref="A2:H16" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="54" xr:uid="{00000000-000C-0000-FFFF-FFFF35000000}" name="Tab2" displayName="Tab2__53" ref="A2:H16" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="97" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="96" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="95" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="94" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="93" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="92" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="91" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="90" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-3500-000001000000}" name="Country" dataDxfId="97" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-3500-000002000000}" name="unit" dataDxfId="96" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-3500-000003000000}" name="2016" dataDxfId="95" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-3500-000004000000}" name="2017" dataDxfId="94" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-3500-000005000000}" name="2018" dataDxfId="93" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-3500-000006000000}" name="2019" dataDxfId="92" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-3500-000007000000}" name="2020" dataDxfId="91" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-3500-000008000000}" name="data source" dataDxfId="90" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table55.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="55" name="Tab2" displayName="Tab2__54" ref="A2:H22" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="55" xr:uid="{00000000-000C-0000-FFFF-FFFF36000000}" name="Tab2" displayName="Tab2__54" ref="A2:H22" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="87" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="86" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="85" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="84" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="83" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="82" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="81" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="80" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-3600-000001000000}" name="Country" dataDxfId="87" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-3600-000002000000}" name="unit" dataDxfId="86" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-3600-000003000000}" name="2016" dataDxfId="85" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-3600-000004000000}" name="2017" dataDxfId="84" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-3600-000005000000}" name="2018" dataDxfId="83" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-3600-000006000000}" name="2019" dataDxfId="82" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-3600-000007000000}" name="2020" dataDxfId="81" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-3600-000008000000}" name="data source" dataDxfId="80" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table56.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="56" name="Tab2" displayName="Tab2__55" ref="A2:H58" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="56" xr:uid="{00000000-000C-0000-FFFF-FFFF37000000}" name="Tab2" displayName="Tab2__55" ref="A2:H58" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="77" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="76" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="75" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="74" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="73" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="72" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="71" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="70" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-3700-000001000000}" name="Country" dataDxfId="77" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-3700-000002000000}" name="unit" dataDxfId="76" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-3700-000003000000}" name="2016" dataDxfId="75" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-3700-000004000000}" name="2017" dataDxfId="74" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-3700-000005000000}" name="2018" dataDxfId="73" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-3700-000006000000}" name="2019" dataDxfId="72" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-3700-000007000000}" name="2020" dataDxfId="71" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-3700-000008000000}" name="data source" dataDxfId="70" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table57.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="57" name="Tab2" displayName="Tab2__56" ref="A2:H25" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="57" xr:uid="{00000000-000C-0000-FFFF-FFFF38000000}" name="Tab2" displayName="Tab2__56" ref="A2:H25" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="67" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="66" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="65" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="64" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="63" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="62" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="61" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="60" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-3800-000001000000}" name="Country" dataDxfId="67" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-3800-000002000000}" name="unit" dataDxfId="66" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-3800-000003000000}" name="2016" dataDxfId="65" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-3800-000004000000}" name="2017" dataDxfId="64" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-3800-000005000000}" name="2018" dataDxfId="63" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-3800-000006000000}" name="2019" dataDxfId="62" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-3800-000007000000}" name="2020" dataDxfId="61" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-3800-000008000000}" name="data source" dataDxfId="60" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table58.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="58" name="Tab2" displayName="Tab2__57" ref="A2:H33" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="58" xr:uid="{00000000-000C-0000-FFFF-FFFF39000000}" name="Tab2" displayName="Tab2__57" ref="A2:H33" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="57" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="56" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="55" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="54" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="53" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="52" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="51" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="50" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-3900-000001000000}" name="Country" dataDxfId="57" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-3900-000002000000}" name="unit" dataDxfId="56" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-3900-000003000000}" name="2016" dataDxfId="55" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-3900-000004000000}" name="2017" dataDxfId="54" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-3900-000005000000}" name="2018" dataDxfId="53" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-3900-000006000000}" name="2019" dataDxfId="52" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-3900-000007000000}" name="2020" dataDxfId="51" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-3900-000008000000}" name="data source" dataDxfId="50" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table59.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="59" name="Tab2" displayName="Tab2__58" ref="A2:H96" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="59" xr:uid="{00000000-000C-0000-FFFF-FFFF3A000000}" name="Tab2" displayName="Tab2__58" ref="A2:H96" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="47" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="46" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="45" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="44" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="43" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="42" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="41" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="40" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-3A00-000001000000}" name="Country" dataDxfId="47" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-3A00-000002000000}" name="unit" dataDxfId="46" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-3A00-000003000000}" name="2016" dataDxfId="45" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-3A00-000004000000}" name="2017" dataDxfId="44" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-3A00-000005000000}" name="2018" dataDxfId="43" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-3A00-000006000000}" name="2019" dataDxfId="42" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-3A00-000007000000}" name="2020" dataDxfId="41" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-3A00-000008000000}" name="data source" dataDxfId="40" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tab2" displayName="Tab2__5" ref="A2:H33" totalsRowShown="0" headerRowDxfId="579" dataDxfId="578" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tab2" displayName="Tab2__5" ref="A2:H33" totalsRowShown="0" headerRowDxfId="579" dataDxfId="578" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="577" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="576" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="575" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="574" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="573" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="572" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="571" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="570" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Country" dataDxfId="577" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="unit" dataDxfId="576" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="2016" dataDxfId="575" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="2017" dataDxfId="574" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="2018" dataDxfId="573" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="2019" dataDxfId="572" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="2020" dataDxfId="571" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="data source" dataDxfId="570" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table60.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="62" name="Tab2" displayName="Tab2__61" ref="A2:H106" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="62" xr:uid="{00000000-000C-0000-FFFF-FFFF3B000000}" name="Tab2" displayName="Tab2__61" ref="A2:H106" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="37" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="36" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="35" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="34" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="33" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="32" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="31" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="30" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-3B00-000001000000}" name="Country" dataDxfId="37" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-3B00-000002000000}" name="unit" dataDxfId="36" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-3B00-000003000000}" name="2016" dataDxfId="35" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-3B00-000004000000}" name="2017" dataDxfId="34" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-3B00-000005000000}" name="2018" dataDxfId="33" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-3B00-000006000000}" name="2019" dataDxfId="32" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-3B00-000007000000}" name="2020" dataDxfId="31" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-3B00-000008000000}" name="data source" dataDxfId="30" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table61.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="60" name="Tab2" displayName="Tab2__59" ref="A2:H5" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="60" xr:uid="{00000000-000C-0000-FFFF-FFFF3C000000}" name="Tab2" displayName="Tab2__59" ref="A2:H5" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="27" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="26" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="25" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="24" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="23" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="22" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="21" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="20" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-3C00-000001000000}" name="Country" dataDxfId="27" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-3C00-000002000000}" name="unit" dataDxfId="26" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-3C00-000003000000}" name="2016" dataDxfId="25" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-3C00-000004000000}" name="2017" dataDxfId="24" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-3C00-000005000000}" name="2018" dataDxfId="23" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-3C00-000006000000}" name="2019" dataDxfId="22" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-3C00-000007000000}" name="2020" dataDxfId="21" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-3C00-000008000000}" name="data source" dataDxfId="20" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table62.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="61" name="Tab2" displayName="Tab2__60" ref="A2:H9" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="61" xr:uid="{00000000-000C-0000-FFFF-FFFF3D000000}" name="Tab2" displayName="Tab2__60" ref="A2:H9" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="17" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="16" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="15" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="14" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="13" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="12" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="11" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="10" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-3D00-000001000000}" name="Country" dataDxfId="17" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-3D00-000002000000}" name="unit" dataDxfId="16" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-3D00-000003000000}" name="2016" dataDxfId="15" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-3D00-000004000000}" name="2017" dataDxfId="14" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-3D00-000005000000}" name="2018" dataDxfId="13" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-3D00-000006000000}" name="2019" dataDxfId="12" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-3D00-000007000000}" name="2020" dataDxfId="11" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-3D00-000008000000}" name="data source" dataDxfId="10" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table63.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="63" name="Tab2" displayName="Tab2__62" ref="A2:H20" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="63" xr:uid="{00000000-000C-0000-FFFF-FFFF3E000000}" name="Tab2" displayName="Tab2__62" ref="A2:H20" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="7" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="6" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="5" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="4" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="3" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="2" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="1" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="0" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-3E00-000001000000}" name="Country" dataDxfId="7" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-3E00-000002000000}" name="unit" dataDxfId="6" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-3E00-000003000000}" name="2016" dataDxfId="5" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-3E00-000004000000}" name="2017" dataDxfId="4" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-3E00-000005000000}" name="2018" dataDxfId="3" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-3E00-000006000000}" name="2019" dataDxfId="2" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-3E00-000007000000}" name="2020" dataDxfId="1" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-3E00-000008000000}" name="data source" dataDxfId="0" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tab2" displayName="Tab2__6" ref="A2:H14" totalsRowShown="0" headerRowDxfId="569" dataDxfId="568" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Tab2" displayName="Tab2__6" ref="A2:H14" totalsRowShown="0" headerRowDxfId="569" dataDxfId="568" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="567" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="566" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="565" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="564" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="563" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="562" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="561" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="560" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Country" dataDxfId="567" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="unit" dataDxfId="566" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="2016" dataDxfId="565" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="2017" dataDxfId="564" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="2018" dataDxfId="563" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="2019" dataDxfId="562" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="2020" dataDxfId="561" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="data source" dataDxfId="560" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tab2" displayName="Tab2__7" ref="A2:H15" totalsRowShown="0" headerRowDxfId="559" dataDxfId="558" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Tab2" displayName="Tab2__7" ref="A2:H15" totalsRowShown="0" headerRowDxfId="559" dataDxfId="558" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="557" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="556" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="555" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="554" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="553" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="552" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="551" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="550" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Country" dataDxfId="557" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="unit" dataDxfId="556" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="2016" dataDxfId="555" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="2017" dataDxfId="554" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="2018" dataDxfId="553" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="2019" dataDxfId="552" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="2020" dataDxfId="551" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="data source" dataDxfId="550" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tab2" displayName="Tab2__8" ref="A2:H26" totalsRowShown="0" headerRowDxfId="549" dataDxfId="548" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tab2" displayName="Tab2__8" ref="A2:H26" totalsRowShown="0" headerRowDxfId="549" dataDxfId="548" headerRowCellStyle="Tabelle Kopf" dataCellStyle="Tabelle allgemein">
   <tableColumns count="8">
-    <tableColumn id="1" name="Country" dataDxfId="547" dataCellStyle="Tabelle 1Spalte"/>
-    <tableColumn id="2" name="unit" dataDxfId="546" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="3" name="2016" dataDxfId="545" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="4" name="2017" dataDxfId="544" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="5" name="2018" dataDxfId="543" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="6" name="2019" dataDxfId="542" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="7" name="2020" dataDxfId="541" dataCellStyle="Tabelle allgemein"/>
-    <tableColumn id="8" name="data source" dataDxfId="540" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Country" dataDxfId="547" dataCellStyle="Tabelle 1Spalte"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="unit" dataDxfId="546" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="2016" dataDxfId="545" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="2017" dataDxfId="544" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="2018" dataDxfId="543" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="2019" dataDxfId="542" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="2020" dataDxfId="541" dataCellStyle="Tabelle allgemein"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="data source" dataDxfId="540" dataCellStyle="Tabelle allgemein"/>
   </tableColumns>
   <tableStyleInfo name="WMD" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -10136,6 +10150,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -10171,6 +10202,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -10346,15 +10394,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle4">
     <tabColor indexed="10"/>
   </sheetPr>
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -11851,7 +11899,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Tabelle13">
     <tabColor indexed="10"/>
   </sheetPr>
@@ -11859,7 +11907,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -12585,7 +12633,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Tabelle14">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -12595,7 +12643,7 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -12827,7 +12875,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr codeName="Tabelle15">
     <tabColor indexed="17"/>
   </sheetPr>
@@ -12837,7 +12885,7 @@
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -13983,7 +14031,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Tabelle16">
     <tabColor indexed="17"/>
   </sheetPr>
@@ -13993,7 +14041,7 @@
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -14593,7 +14641,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr codeName="Tabelle17">
     <tabColor indexed="17"/>
   </sheetPr>
@@ -14603,7 +14651,7 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -14917,7 +14965,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr codeName="Tabelle18">
     <tabColor indexed="17"/>
   </sheetPr>
@@ -14927,7 +14975,7 @@
       <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -15886,7 +15934,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <tabColor indexed="17"/>
   </sheetPr>
@@ -15896,7 +15944,7 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.25" style="3" customWidth="1"/>
     <col min="2" max="16384" width="10.875" style="3"/>
@@ -16178,7 +16226,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr codeName="Tabelle19">
     <tabColor indexed="17"/>
   </sheetPr>
@@ -16188,7 +16236,7 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -16555,7 +16603,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr codeName="Tabelle20">
     <tabColor indexed="17"/>
   </sheetPr>
@@ -16565,7 +16613,7 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -17139,7 +17187,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr codeName="Tabelle21">
     <tabColor indexed="17"/>
   </sheetPr>
@@ -17149,7 +17197,7 @@
       <selection activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -18785,7 +18833,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Tabelle5">
     <tabColor indexed="10"/>
   </sheetPr>
@@ -18795,7 +18843,7 @@
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -19417,7 +19465,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr codeName="Tabelle22">
     <tabColor indexed="17"/>
   </sheetPr>
@@ -19427,7 +19475,7 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -19663,7 +19711,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr codeName="Tabelle23">
     <tabColor indexed="17"/>
   </sheetPr>
@@ -19673,7 +19721,7 @@
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -19883,7 +19931,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr>
     <tabColor indexed="17"/>
   </sheetPr>
@@ -19893,7 +19941,7 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="10.875" style="3"/>
   </cols>
@@ -20226,7 +20274,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <sheetPr codeName="Tabelle24">
     <tabColor indexed="17"/>
   </sheetPr>
@@ -20236,7 +20284,7 @@
       <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.875" style="3" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" customWidth="1"/>
@@ -21586,7 +21634,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <sheetPr codeName="Tabelle25">
     <tabColor indexed="17"/>
   </sheetPr>
@@ -21596,7 +21644,7 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -21984,7 +22032,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr codeName="Tabelle26">
     <tabColor indexed="17"/>
   </sheetPr>
@@ -21994,7 +22042,7 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -22334,7 +22382,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <sheetPr codeName="Tabelle27">
     <tabColor indexed="17"/>
   </sheetPr>
@@ -22344,7 +22392,7 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -22656,7 +22704,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <sheetPr codeName="Tabelle28">
     <tabColor indexed="17"/>
   </sheetPr>
@@ -22666,7 +22714,7 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.25" style="3" customWidth="1"/>
@@ -22954,7 +23002,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <sheetPr codeName="Tabelle29">
     <tabColor indexed="17"/>
   </sheetPr>
@@ -22964,7 +23012,7 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -23512,7 +23560,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <sheetPr codeName="Tabelle30">
     <tabColor indexed="17"/>
   </sheetPr>
@@ -23522,7 +23570,7 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -23810,7 +23858,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Tabelle6">
     <tabColor indexed="10"/>
   </sheetPr>
@@ -23820,7 +23868,7 @@
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -24446,7 +24494,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <sheetPr codeName="Tabelle31">
     <tabColor indexed="17"/>
   </sheetPr>
@@ -24456,7 +24504,7 @@
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -25178,7 +25226,7 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <sheetPr codeName="Tabelle32">
     <tabColor indexed="17"/>
   </sheetPr>
@@ -25188,7 +25236,7 @@
       <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -26724,17 +26772,17 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <sheetPr codeName="Tabelle33">
     <tabColor indexed="28"/>
   </sheetPr>
   <dimension ref="A1:H103"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
+    <sheetView topLeftCell="A87" workbookViewId="0">
       <selection activeCell="K98" sqref="K98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="3" bestFit="1" customWidth="1"/>
@@ -29410,17 +29458,17 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <sheetPr codeName="Tabelle34">
     <tabColor indexed="28"/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="J3" sqref="J3:J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="3" bestFit="1" customWidth="1"/>
@@ -29429,7 +29477,7 @@
     <col min="9" max="16384" width="10.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>172</v>
       </c>
@@ -29441,7 +29489,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>89</v>
       </c>
@@ -29467,7 +29515,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -29492,8 +29540,16 @@
       <c r="H3" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3" s="3">
+        <f>RANK(Tab2__30[[#This Row],[2016]],$C$3:$C$13)</f>
+        <v>8</v>
+      </c>
+      <c r="K3" s="3">
+        <f>RANK(Tab2__30[[#This Row],[2017]],$D$3:$D$13)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -29518,8 +29574,16 @@
       <c r="H4" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4" s="3">
+        <f>RANK(Tab2__30[[#This Row],[2016]],$C$3:$C$13)</f>
+        <v>3</v>
+      </c>
+      <c r="K4" s="3">
+        <f>RANK(Tab2__30[[#This Row],[2017]],$D$3:$D$13)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -29544,8 +29608,16 @@
       <c r="H5" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5" s="3">
+        <f>RANK(Tab2__30[[#This Row],[2016]],$C$3:$C$13)</f>
+        <v>6</v>
+      </c>
+      <c r="K5" s="3">
+        <f>RANK(Tab2__30[[#This Row],[2017]],$D$3:$D$13)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
@@ -29570,8 +29642,16 @@
       <c r="H6" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6" s="3">
+        <f>RANK(Tab2__30[[#This Row],[2016]],$C$3:$C$13)</f>
+        <v>7</v>
+      </c>
+      <c r="K6" s="3">
+        <f>RANK(Tab2__30[[#This Row],[2017]],$D$3:$D$13)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>78</v>
       </c>
@@ -29596,8 +29676,16 @@
       <c r="H7" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7" s="3">
+        <f>RANK(Tab2__30[[#This Row],[2016]],$C$3:$C$13)</f>
+        <v>9</v>
+      </c>
+      <c r="K7" s="3">
+        <f>RANK(Tab2__30[[#This Row],[2017]],$D$3:$D$13)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>169</v>
       </c>
@@ -29622,8 +29710,16 @@
       <c r="H8" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8" s="3">
+        <f>RANK(Tab2__30[[#This Row],[2016]],$C$3:$C$13)</f>
+        <v>1</v>
+      </c>
+      <c r="K8" s="3">
+        <f>RANK(Tab2__30[[#This Row],[2017]],$D$3:$D$13)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>117</v>
       </c>
@@ -29648,8 +29744,16 @@
       <c r="H9" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J9" s="3">
+        <f>RANK(Tab2__30[[#This Row],[2016]],$C$3:$C$13)</f>
+        <v>10</v>
+      </c>
+      <c r="K9" s="3">
+        <f>RANK(Tab2__30[[#This Row],[2017]],$D$3:$D$13)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>38</v>
       </c>
@@ -29674,8 +29778,16 @@
       <c r="H10" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J10" s="3">
+        <f>RANK(Tab2__30[[#This Row],[2016]],$C$3:$C$13)</f>
+        <v>2</v>
+      </c>
+      <c r="K10" s="3">
+        <f>RANK(Tab2__30[[#This Row],[2017]],$D$3:$D$13)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>46</v>
       </c>
@@ -29700,8 +29812,16 @@
       <c r="H11" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J11" s="3">
+        <f>RANK(Tab2__30[[#This Row],[2016]],$C$3:$C$13)</f>
+        <v>4</v>
+      </c>
+      <c r="K11" s="3">
+        <f>RANK(Tab2__30[[#This Row],[2017]],$D$3:$D$13)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>76</v>
       </c>
@@ -29722,8 +29842,16 @@
       <c r="H12" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J12" s="3" t="e">
+        <f>RANK(Tab2__30[[#This Row],[2016]],$C$3:$C$13)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K12" s="3" t="e">
+        <f>RANK(Tab2__30[[#This Row],[2017]],$D$3:$D$13)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>58</v>
       </c>
@@ -29748,8 +29876,16 @@
       <c r="H13" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J13" s="3">
+        <f>RANK(Tab2__30[[#This Row],[2016]],$C$3:$C$13)</f>
+        <v>5</v>
+      </c>
+      <c r="K13" s="3">
+        <f>RANK(Tab2__30[[#This Row],[2017]],$D$3:$D$13)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>50</v>
       </c>
@@ -29782,17 +29918,17 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <sheetPr codeName="Tabelle35">
     <tabColor indexed="28"/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="K3" sqref="K3:K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="3" bestFit="1" customWidth="1"/>
@@ -29801,7 +29937,7 @@
     <col min="9" max="16384" width="10.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>172</v>
       </c>
@@ -29813,7 +29949,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>89</v>
       </c>
@@ -29839,7 +29975,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -29864,8 +30000,16 @@
       <c r="H3" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3" s="3">
+        <f>RANK(Tab2__31[[#This Row],[2016]],$C$3:$C$13)</f>
+        <v>9</v>
+      </c>
+      <c r="K3" s="3">
+        <f>RANK(Tab2__31[[#This Row],[2017]],$D$3:$D$13)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -29890,8 +30034,16 @@
       <c r="H4" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4" s="3">
+        <f>RANK(Tab2__31[[#This Row],[2016]],$C$3:$C$13)</f>
+        <v>4</v>
+      </c>
+      <c r="K4" s="3">
+        <f>RANK(Tab2__31[[#This Row],[2017]],$D$3:$D$13)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -29916,8 +30068,16 @@
       <c r="H5" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5" s="3">
+        <f>RANK(Tab2__31[[#This Row],[2016]],$C$3:$C$13)</f>
+        <v>6</v>
+      </c>
+      <c r="K5" s="3">
+        <f>RANK(Tab2__31[[#This Row],[2017]],$D$3:$D$13)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -29942,8 +30102,16 @@
       <c r="H6" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6" s="3">
+        <f>RANK(Tab2__31[[#This Row],[2016]],$C$3:$C$13)</f>
+        <v>8</v>
+      </c>
+      <c r="K6" s="3">
+        <f>RANK(Tab2__31[[#This Row],[2017]],$D$3:$D$13)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>52</v>
       </c>
@@ -29968,8 +30136,16 @@
       <c r="H7" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7" s="3">
+        <f>RANK(Tab2__31[[#This Row],[2016]],$C$3:$C$13)</f>
+        <v>7</v>
+      </c>
+      <c r="K7" s="3">
+        <f>RANK(Tab2__31[[#This Row],[2017]],$D$3:$D$13)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>78</v>
       </c>
@@ -29994,8 +30170,16 @@
       <c r="H8" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8" s="3">
+        <f>RANK(Tab2__31[[#This Row],[2016]],$C$3:$C$13)</f>
+        <v>10</v>
+      </c>
+      <c r="K8" s="3">
+        <f>RANK(Tab2__31[[#This Row],[2017]],$D$3:$D$13)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>169</v>
       </c>
@@ -30020,8 +30204,16 @@
       <c r="H9" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J9" s="3">
+        <f>RANK(Tab2__31[[#This Row],[2016]],$C$3:$C$13)</f>
+        <v>2</v>
+      </c>
+      <c r="K9" s="3">
+        <f>RANK(Tab2__31[[#This Row],[2017]],$D$3:$D$13)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>117</v>
       </c>
@@ -30046,8 +30238,16 @@
       <c r="H10" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J10" s="3">
+        <f>RANK(Tab2__31[[#This Row],[2016]],$C$3:$C$13)</f>
+        <v>11</v>
+      </c>
+      <c r="K10" s="3">
+        <f>RANK(Tab2__31[[#This Row],[2017]],$D$3:$D$13)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
@@ -30072,8 +30272,16 @@
       <c r="H11" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J11" s="3">
+        <f>RANK(Tab2__31[[#This Row],[2016]],$C$3:$C$13)</f>
+        <v>1</v>
+      </c>
+      <c r="K11" s="3">
+        <f>RANK(Tab2__31[[#This Row],[2017]],$D$3:$D$13)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
@@ -30098,8 +30306,16 @@
       <c r="H12" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J12" s="3">
+        <f>RANK(Tab2__31[[#This Row],[2016]],$C$3:$C$13)</f>
+        <v>5</v>
+      </c>
+      <c r="K12" s="3">
+        <f>RANK(Tab2__31[[#This Row],[2017]],$D$3:$D$13)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>58</v>
       </c>
@@ -30124,8 +30340,16 @@
       <c r="H13" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J13" s="3">
+        <f>RANK(Tab2__31[[#This Row],[2016]],$C$3:$C$13)</f>
+        <v>3</v>
+      </c>
+      <c r="K13" s="3">
+        <f>RANK(Tab2__31[[#This Row],[2017]],$D$3:$D$13)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
@@ -30158,7 +30382,7 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <sheetPr codeName="Tabelle36">
     <tabColor indexed="28"/>
   </sheetPr>
@@ -30168,7 +30392,7 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="3" bestFit="1" customWidth="1"/>
@@ -30378,17 +30602,17 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <sheetPr codeName="Tabelle37">
     <tabColor indexed="28"/>
   </sheetPr>
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="K63" sqref="K63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="3" bestFit="1" customWidth="1"/>
@@ -30397,7 +30621,7 @@
     <col min="9" max="16384" width="10.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>172</v>
       </c>
@@ -30409,7 +30633,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>89</v>
       </c>
@@ -30435,7 +30659,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -30460,8 +30684,12 @@
       <c r="H3" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -30486,8 +30714,12 @@
       <c r="H4" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>75</v>
       </c>
@@ -30512,8 +30744,12 @@
       <c r="H5" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -30538,8 +30774,12 @@
       <c r="H6" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -30564,8 +30804,12 @@
       <c r="H7" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>84</v>
       </c>
@@ -30590,8 +30834,12 @@
       <c r="H8" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -30616,8 +30864,12 @@
       <c r="H9" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J9" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>64</v>
       </c>
@@ -30642,8 +30894,12 @@
       <c r="H10" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J10" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>65</v>
       </c>
@@ -30668,8 +30924,12 @@
       <c r="H11" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J11" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -30694,8 +30954,12 @@
       <c r="H12" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J12" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -30720,8 +30984,12 @@
       <c r="H13" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J13" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -30746,8 +31014,12 @@
       <c r="H14" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J14" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -30772,8 +31044,12 @@
       <c r="H15" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J15" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>60</v>
       </c>
@@ -30798,8 +31074,12 @@
       <c r="H16" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J16" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>66</v>
       </c>
@@ -30824,8 +31104,12 @@
       <c r="H17" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J17" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>115</v>
       </c>
@@ -30850,8 +31134,12 @@
       <c r="H18" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J18" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>77</v>
       </c>
@@ -30876,8 +31164,12 @@
       <c r="H19" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J19" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>123</v>
       </c>
@@ -30902,8 +31194,12 @@
       <c r="H20" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J20" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>116</v>
       </c>
@@ -30928,8 +31224,12 @@
       <c r="H21" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J21" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>81</v>
       </c>
@@ -30954,8 +31254,12 @@
       <c r="H22" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J22" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>108</v>
       </c>
@@ -30980,8 +31284,12 @@
       <c r="H23" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J23" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
@@ -31006,8 +31314,12 @@
       <c r="H24" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J24" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>68</v>
       </c>
@@ -31032,8 +31344,12 @@
       <c r="H25" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J25" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>14</v>
       </c>
@@ -31058,8 +31374,12 @@
       <c r="H26" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J26" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>69</v>
       </c>
@@ -31084,8 +31404,12 @@
       <c r="H27" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J27" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>53</v>
       </c>
@@ -31110,8 +31434,12 @@
       <c r="H28" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J28" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>15</v>
       </c>
@@ -31136,8 +31464,12 @@
       <c r="H29" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J29" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>105</v>
       </c>
@@ -31162,8 +31494,12 @@
       <c r="H30" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J30" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>16</v>
       </c>
@@ -31188,8 +31524,12 @@
       <c r="H31" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J31" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>17</v>
       </c>
@@ -31214,8 +31554,12 @@
       <c r="H32" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J32" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>18</v>
       </c>
@@ -31240,8 +31584,12 @@
       <c r="H33" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J33" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>118</v>
       </c>
@@ -31266,8 +31614,12 @@
       <c r="H34" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J34" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>97</v>
       </c>
@@ -31292,8 +31644,12 @@
       <c r="H35" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J35" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>19</v>
       </c>
@@ -31318,8 +31674,12 @@
       <c r="H36" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J36" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
@@ -31344,8 +31704,12 @@
       <c r="H37" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J37" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>22</v>
       </c>
@@ -31370,8 +31734,12 @@
       <c r="H38" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J38" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>86</v>
       </c>
@@ -31396,8 +31764,12 @@
       <c r="H39" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J39" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>23</v>
       </c>
@@ -31422,8 +31794,12 @@
       <c r="H40" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J40" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>25</v>
       </c>
@@ -31448,8 +31824,12 @@
       <c r="H41" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J41" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>125</v>
       </c>
@@ -31474,8 +31854,12 @@
       <c r="H42" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J42" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>27</v>
       </c>
@@ -31500,8 +31884,12 @@
       <c r="H43" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J43" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>28</v>
       </c>
@@ -31526,8 +31914,12 @@
       <c r="H44" s="2" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J44" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>29</v>
       </c>
@@ -31552,8 +31944,12 @@
       <c r="H45" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J45" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>72</v>
       </c>
@@ -31578,8 +31974,12 @@
       <c r="H46" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J46" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>30</v>
       </c>
@@ -31604,8 +32004,12 @@
       <c r="H47" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J47" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>126</v>
       </c>
@@ -31630,8 +32034,12 @@
       <c r="H48" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J48" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>127</v>
       </c>
@@ -31656,8 +32064,12 @@
       <c r="H49" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J49" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>180</v>
       </c>
@@ -31682,8 +32094,12 @@
       <c r="H50" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J50" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>128</v>
       </c>
@@ -31704,8 +32120,12 @@
       <c r="H51" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J51" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>57</v>
       </c>
@@ -31730,8 +32150,12 @@
       <c r="H52" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J52" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>34</v>
       </c>
@@ -31756,8 +32180,12 @@
       <c r="H53" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J53" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>35</v>
       </c>
@@ -31782,8 +32210,12 @@
       <c r="H54" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J54" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>78</v>
       </c>
@@ -31808,8 +32240,12 @@
       <c r="H55" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J55" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>87</v>
       </c>
@@ -31834,8 +32270,12 @@
       <c r="H56" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J56" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>73</v>
       </c>
@@ -31860,8 +32300,12 @@
       <c r="H57" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J57" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>169</v>
       </c>
@@ -31886,8 +32330,12 @@
       <c r="H58" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J58" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>36</v>
       </c>
@@ -31912,8 +32360,12 @@
       <c r="H59" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J59" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>74</v>
       </c>
@@ -31938,8 +32390,12 @@
       <c r="H60" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J60" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>117</v>
       </c>
@@ -31964,8 +32420,12 @@
       <c r="H61" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J61" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>101</v>
       </c>
@@ -31990,8 +32450,12 @@
       <c r="H62" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J62" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>38</v>
       </c>
@@ -32016,8 +32480,12 @@
       <c r="H63" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J63" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>79</v>
       </c>
@@ -32042,8 +32510,12 @@
       <c r="H64" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J64" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>39</v>
       </c>
@@ -32068,8 +32540,12 @@
       <c r="H65" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J65" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>40</v>
       </c>
@@ -32094,8 +32570,12 @@
       <c r="H66" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J66" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>103</v>
       </c>
@@ -32120,8 +32600,12 @@
       <c r="H67" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J67" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>114</v>
       </c>
@@ -32146,8 +32630,12 @@
       <c r="H68" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J68" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>41</v>
       </c>
@@ -32172,8 +32660,12 @@
       <c r="H69" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J69" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>43</v>
       </c>
@@ -32198,8 +32690,12 @@
       <c r="H70" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J70" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>88</v>
       </c>
@@ -32224,8 +32720,12 @@
       <c r="H71" s="2" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J71" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
         <v>46</v>
       </c>
@@ -32250,8 +32750,12 @@
       <c r="H72" s="9" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J72" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
         <v>76</v>
       </c>
@@ -32276,8 +32780,12 @@
       <c r="H73" s="9" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J73" s="3">
+        <f>RANK(Tab2__33[[#This Row],[2016]],$C$3:$C$73)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
         <v>50</v>
       </c>
@@ -32310,7 +32818,7 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <sheetPr codeName="Tabelle38">
     <tabColor indexed="18"/>
   </sheetPr>
@@ -32320,7 +32828,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -32530,7 +33038,7 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <sheetPr codeName="Tabelle39">
     <tabColor indexed="18"/>
   </sheetPr>
@@ -32540,7 +33048,7 @@
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -33452,7 +33960,7 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <sheetPr codeName="Tabelle40">
     <tabColor indexed="18"/>
   </sheetPr>
@@ -33462,7 +33970,7 @@
       <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -34840,7 +35348,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Tabelle7">
     <tabColor indexed="10"/>
   </sheetPr>
@@ -34850,7 +35358,7 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -35912,7 +36420,7 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <sheetPr codeName="Tabelle41">
     <tabColor indexed="18"/>
   </sheetPr>
@@ -35922,7 +36430,7 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -36262,7 +36770,7 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <sheetPr codeName="Tabelle42">
     <tabColor indexed="18"/>
   </sheetPr>
@@ -36272,7 +36780,7 @@
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="3" bestFit="1" customWidth="1"/>
@@ -36922,7 +37430,7 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
   <sheetPr codeName="Tabelle43">
     <tabColor indexed="18"/>
   </sheetPr>
@@ -36930,7 +37438,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="3" bestFit="1" customWidth="1"/>
@@ -37580,7 +38088,7 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
   <sheetPr codeName="Tabelle44">
     <tabColor indexed="18"/>
   </sheetPr>
@@ -37590,7 +38098,7 @@
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -38294,7 +38802,7 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
   <sheetPr codeName="Tabelle45">
     <tabColor indexed="18"/>
   </sheetPr>
@@ -38304,7 +38812,7 @@
       <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -39632,7 +40140,7 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
   <sheetPr codeName="Tabelle46">
     <tabColor indexed="18"/>
   </sheetPr>
@@ -39642,7 +40150,7 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -40388,7 +40896,7 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
   <sheetPr codeName="Tabelle47">
     <tabColor indexed="18"/>
   </sheetPr>
@@ -40398,7 +40906,7 @@
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -40992,7 +41500,7 @@
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
   <sheetPr codeName="Tabelle48">
     <tabColor indexed="18"/>
   </sheetPr>
@@ -41002,7 +41510,7 @@
       <selection activeCell="K78" sqref="K78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -43110,7 +43618,7 @@
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
   <sheetPr codeName="Tabelle49">
     <tabColor indexed="18"/>
   </sheetPr>
@@ -43120,7 +43628,7 @@
       <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -44708,7 +45216,7 @@
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
   <sheetPr codeName="Tabelle50">
     <tabColor indexed="18"/>
   </sheetPr>
@@ -44718,7 +45226,7 @@
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -45448,7 +45956,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Tabelle8">
     <tabColor indexed="10"/>
   </sheetPr>
@@ -45458,7 +45966,7 @@
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -45980,7 +46488,7 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
   <sheetPr codeName="Tabelle51">
     <tabColor indexed="18"/>
   </sheetPr>
@@ -45990,7 +46498,7 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -46486,7 +46994,7 @@
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
   <sheetPr codeName="Tabelle52">
     <tabColor indexed="18"/>
   </sheetPr>
@@ -46496,7 +47004,7 @@
       <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -47590,7 +48098,7 @@
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3300-000000000000}">
   <sheetPr codeName="Tabelle53">
     <tabColor indexed="18"/>
   </sheetPr>
@@ -47600,7 +48108,7 @@
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -48116,7 +48624,7 @@
 </file>
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3400-000000000000}">
   <sheetPr codeName="Tabelle54">
     <tabColor indexed="18"/>
   </sheetPr>
@@ -48126,7 +48634,7 @@
       <selection activeCell="E108" sqref="E108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -50832,7 +51340,7 @@
 </file>
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3500-000000000000}">
   <sheetPr codeName="Tabelle55">
     <tabColor indexed="18"/>
   </sheetPr>
@@ -50842,7 +51350,7 @@
       <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -52326,7 +52834,7 @@
 </file>
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3600-000000000000}">
   <sheetPr codeName="Tabelle56">
     <tabColor indexed="18"/>
   </sheetPr>
@@ -52336,7 +52844,7 @@
       <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -53378,7 +53886,7 @@
 </file>
 
 <file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3700-000000000000}">
   <sheetPr codeName="Tabelle57">
     <tabColor indexed="18"/>
   </sheetPr>
@@ -53388,7 +53896,7 @@
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -53806,7 +54314,7 @@
 </file>
 
 <file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3800-000000000000}">
   <sheetPr codeName="Tabelle58">
     <tabColor indexed="18"/>
   </sheetPr>
@@ -53816,7 +54324,7 @@
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -54390,7 +54898,7 @@
 </file>
 
 <file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3900-000000000000}">
   <sheetPr codeName="Tabelle59">
     <tabColor indexed="13"/>
   </sheetPr>
@@ -54400,7 +54908,7 @@
       <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -55910,7 +56418,7 @@
 </file>
 
 <file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3A00-000000000000}">
   <sheetPr codeName="Tabelle60">
     <tabColor indexed="13"/>
   </sheetPr>
@@ -55920,7 +56428,7 @@
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -56572,7 +57080,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Tabelle9">
     <tabColor indexed="10"/>
   </sheetPr>
@@ -56582,7 +57090,7 @@
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -57438,7 +57946,7 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3B00-000000000000}">
   <sheetPr codeName="Tabelle61">
     <tabColor indexed="13"/>
   </sheetPr>
@@ -57448,7 +57956,7 @@
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -58308,7 +58816,7 @@
 </file>
 
 <file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3C00-000000000000}">
   <sheetPr codeName="Tabelle62">
     <tabColor indexed="13"/>
   </sheetPr>
@@ -58318,7 +58826,7 @@
       <selection activeCell="F100" sqref="F100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.875" style="3" bestFit="1" customWidth="1"/>
@@ -60817,7 +61325,7 @@
 </file>
 
 <file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3D00-000000000000}">
   <sheetPr codeName="Tabelle65">
     <tabColor indexed="13"/>
   </sheetPr>
@@ -60827,7 +61335,7 @@
       <selection activeCell="D111" sqref="D111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -63577,7 +64085,7 @@
 </file>
 
 <file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3E00-000000000000}">
   <sheetPr codeName="Tabelle63">
     <tabColor indexed="13"/>
   </sheetPr>
@@ -63587,7 +64095,7 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -63719,7 +64227,7 @@
 </file>
 
 <file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3F00-000000000000}">
   <sheetPr codeName="Tabelle64">
     <tabColor indexed="13"/>
   </sheetPr>
@@ -63729,7 +64237,7 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -63961,7 +64469,7 @@
 </file>
 
 <file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4000-000000000000}">
   <sheetPr codeName="Tabelle66">
     <tabColor indexed="13"/>
   </sheetPr>
@@ -63971,7 +64479,7 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -64493,7 +65001,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Tabelle10">
     <tabColor indexed="10"/>
   </sheetPr>
@@ -64503,7 +65011,7 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -64869,7 +65377,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Tabelle11">
     <tabColor indexed="10"/>
   </sheetPr>
@@ -64879,7 +65387,7 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>
@@ -65271,7 +65779,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Tabelle12">
     <tabColor indexed="10"/>
   </sheetPr>
@@ -65281,7 +65789,7 @@
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.75" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="3" bestFit="1" customWidth="1"/>

</xml_diff>